<commit_message>
All functions are now in PHP script
</commit_message>
<xml_diff>
--- a/Data/ParkirnaMesta.xlsx
+++ b/Data/ParkirnaMesta.xlsx
@@ -343,7 +343,7 @@
     <t>Obdobje</t>
   </si>
   <si>
-    <t>Stanje</t>
+    <t>1(24ur)</t>
   </si>
 </sst>
 </file>
@@ -663,7 +663,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -733,37 +733,11 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -816,11 +790,81 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -866,36 +910,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C6500"/>
       </font>
       <fill>
@@ -931,96 +945,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1332,7 +1256,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1340,12 +1264,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="G1" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,11 +1284,10 @@
     <col min="8" max="15" width="17.7109375" style="5" customWidth="1"/>
     <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.42578125" customWidth="1"/>
-    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="62.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1416,14 +1339,11 @@
       <c r="Q1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="R1" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="S1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
@@ -1473,9 +1393,8 @@
       <c r="Q2" s="1">
         <v>1</v>
       </c>
-      <c r="R2" s="26"/>
-    </row>
-    <row r="3" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1525,9 +1444,8 @@
       <c r="Q3" s="1">
         <v>1</v>
       </c>
-      <c r="R3" s="26"/>
-    </row>
-    <row r="4" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -1577,9 +1495,8 @@
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="26"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1629,9 +1546,8 @@
       <c r="Q5" s="1">
         <v>1</v>
       </c>
-      <c r="R5" s="26"/>
-    </row>
-    <row r="6" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1649,7 +1565,7 @@
         <v>0</v>
       </c>
       <c r="G6" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>82</v>
@@ -1681,9 +1597,8 @@
       <c r="Q6" s="1">
         <v>1</v>
       </c>
-      <c r="R6" s="26"/>
-    </row>
-    <row r="7" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -1733,9 +1648,8 @@
       <c r="Q7" s="1">
         <v>1</v>
       </c>
-      <c r="R7" s="26"/>
-    </row>
-    <row r="8" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -1785,9 +1699,8 @@
       <c r="Q8" s="1">
         <v>1</v>
       </c>
-      <c r="R8" s="26"/>
-    </row>
-    <row r="9" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1837,9 +1750,8 @@
       <c r="Q9" s="1">
         <v>1</v>
       </c>
-      <c r="R9" s="26"/>
-    </row>
-    <row r="10" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -1889,9 +1801,8 @@
       <c r="Q10" s="1">
         <v>1</v>
       </c>
-      <c r="R10" s="26"/>
-    </row>
-    <row r="11" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -1941,9 +1852,8 @@
       <c r="Q11" s="1">
         <v>0.5</v>
       </c>
-      <c r="R11" s="26"/>
-    </row>
-    <row r="12" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1993,9 +1903,8 @@
       <c r="Q12" s="1">
         <v>1</v>
       </c>
-      <c r="R12" s="26"/>
-    </row>
-    <row r="13" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -2045,9 +1954,8 @@
       <c r="Q13" s="1">
         <v>1</v>
       </c>
-      <c r="R13" s="26"/>
-    </row>
-    <row r="14" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -2097,9 +2005,8 @@
       <c r="Q14" s="1">
         <v>1</v>
       </c>
-      <c r="R14" s="26"/>
-    </row>
-    <row r="15" spans="1:19" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:18" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2149,9 +2056,8 @@
       <c r="Q15" s="1">
         <v>1</v>
       </c>
-      <c r="R15" s="26"/>
-    </row>
-    <row r="16" spans="1:19" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:18" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
@@ -2201,9 +2107,8 @@
       <c r="Q16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="26"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
@@ -2253,9 +2158,8 @@
       <c r="Q17" s="1">
         <v>1</v>
       </c>
-      <c r="R17" s="26"/>
-    </row>
-    <row r="18" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -2305,9 +2209,8 @@
       <c r="Q18" s="1">
         <v>1</v>
       </c>
-      <c r="R18" s="26"/>
-    </row>
-    <row r="19" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
@@ -2357,9 +2260,8 @@
       <c r="Q19" s="1">
         <v>1</v>
       </c>
-      <c r="R19" s="26"/>
-    </row>
-    <row r="20" spans="1:19" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:18" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
@@ -2409,9 +2311,8 @@
       <c r="Q20" s="1">
         <v>1</v>
       </c>
-      <c r="R20" s="26"/>
-    </row>
-    <row r="21" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
@@ -2429,7 +2330,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21" s="11" t="s">
         <v>82</v>
@@ -2461,9 +2362,8 @@
       <c r="Q21" s="1">
         <v>0.5</v>
       </c>
-      <c r="R21" s="26"/>
-    </row>
-    <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
@@ -2513,9 +2413,8 @@
       <c r="Q22" s="1">
         <v>1</v>
       </c>
-      <c r="R22" s="26"/>
-    </row>
-    <row r="23" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
@@ -2565,12 +2464,11 @@
       <c r="Q23" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>43</v>
       </c>
@@ -2620,9 +2518,8 @@
       <c r="Q24" s="1">
         <v>0.5</v>
       </c>
-      <c r="R24" s="26"/>
-    </row>
-    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2672,9 +2569,8 @@
       <c r="Q25" s="1">
         <v>0.5</v>
       </c>
-      <c r="R25" s="26"/>
-    </row>
-    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -2724,9 +2620,8 @@
       <c r="Q26" s="1">
         <v>0.5</v>
       </c>
-      <c r="R26" s="26"/>
-    </row>
-    <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -2776,9 +2671,8 @@
       <c r="Q27" s="1">
         <v>0.5</v>
       </c>
-      <c r="R27" s="26"/>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>51</v>
       </c>
@@ -2828,9 +2722,8 @@
       <c r="Q28" s="1">
         <v>1</v>
       </c>
-      <c r="R28" s="26"/>
-    </row>
-    <row r="29" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>53</v>
       </c>
@@ -2880,12 +2773,11 @@
       <c r="Q29" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1" t="s">
+      <c r="R29" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>55</v>
       </c>
@@ -2935,12 +2827,11 @@
       <c r="Q30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1" t="s">
+      <c r="R30" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -2990,12 +2881,11 @@
       <c r="Q31" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1" t="s">
+      <c r="R31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>60</v>
       </c>
@@ -3045,9 +2935,8 @@
       <c r="Q32" s="1">
         <v>1</v>
       </c>
-      <c r="R32" s="26"/>
-    </row>
-    <row r="33" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>62</v>
       </c>
@@ -3097,9 +2986,8 @@
       <c r="Q33" s="1">
         <v>1</v>
       </c>
-      <c r="R33" s="26"/>
-    </row>
-    <row r="34" spans="1:19" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:18" ht="29.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>64</v>
       </c>
@@ -3149,9 +3037,8 @@
       <c r="Q34" s="1">
         <v>0.5</v>
       </c>
-      <c r="R34" s="26"/>
-    </row>
-    <row r="35" spans="1:19" ht="72" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:18" ht="72" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>66</v>
       </c>
@@ -3169,7 +3056,7 @@
         <v>0</v>
       </c>
       <c r="G35" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H35" s="11" t="s">
         <v>82</v>
@@ -3195,18 +3082,17 @@
       <c r="O35" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="P35" s="14">
-        <v>1</v>
+      <c r="P35" s="14" t="s">
+        <v>107</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1" t="s">
+      <c r="R35" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>69</v>
       </c>
@@ -3256,9 +3142,8 @@
       <c r="Q36" s="1">
         <v>0.5</v>
       </c>
-      <c r="R36" s="26"/>
-    </row>
-    <row r="37" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>71</v>
       </c>
@@ -3308,9 +3193,8 @@
       <c r="Q37" s="1">
         <v>0.5</v>
       </c>
-      <c r="R37" s="26"/>
-    </row>
-    <row r="38" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>73</v>
       </c>
@@ -3360,9 +3244,8 @@
       <c r="Q38" s="1">
         <v>0.5</v>
       </c>
-      <c r="R38" s="26"/>
-    </row>
-    <row r="39" spans="1:19" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:18" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>75</v>
       </c>
@@ -3380,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="G39" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H39" s="11" t="s">
         <v>82</v>
@@ -3412,39 +3295,43 @@
       <c r="Q39" s="1">
         <v>0.5</v>
       </c>
-      <c r="R39" s="26"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="S1 G1:G6 G9:G1048576 I1:O1048576">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="equal">
+  <conditionalFormatting sqref="R1 G1:G6 G9:G34 I1:O1048576 G36:G1048576">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>$O$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1:G6 G9:G1048576">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+  <conditionalFormatting sqref="G1:G6 G9:G34 G36:G1048576">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>$G$35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>$G$23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G8">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>$G$35</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$G$23</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>$G$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G8">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>$O$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39 G6 G21">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>